<commit_message>
Versión de curvas ajustadas - path 3
</commit_message>
<xml_diff>
--- a/project/Lectura Sensor/Tabla de Valores.xlsx
+++ b/project/Lectura Sensor/Tabla de Valores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utpac-my.sharepoint.com/personal/armando_almengor_utp_ac_pa/Documents/Universidad/Trabajo de Graduación/Mecatrónica/Proyecto Final/Lectura Sensor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive - Universidad Tecnológica de Panamá\Documents\Proyectos\Acádemicos\UPV\SEM_B-2021\MEC\MATLAB\upv_mechatronics--matlab\project\Lectura Sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="467" documentId="13_ncr:1_{2EEE4CDC-63EF-4E34-B2E4-20CC1611E3FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0740EFCC-701F-4C60-8FE2-71F693905644}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96831B3F-4957-47E2-9F35-54DAA1A3572B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2124" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="5" xr2:uid="{52C5606A-8AC3-4B61-9351-7CD081ABF504}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{52C5606A-8AC3-4B61-9351-7CD081ABF504}"/>
   </bookViews>
   <sheets>
     <sheet name="Alexander - Juan" sheetId="1" state="hidden" r:id="rId1"/>
@@ -32525,10 +32525,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F55C6B-8660-48F2-AA7F-2395DA23B8BC}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32595,6 +32595,39 @@
         <v>8</v>
       </c>
       <c r="I2">
+        <v>0.12130000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>F3-E3</f>
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <f>G3*A3</f>
+        <v>190</v>
+      </c>
+      <c r="C3">
+        <f>H3-I3*B3</f>
+        <v>-15.047000000000001</v>
+      </c>
+      <c r="D3">
+        <f>H3+I3*B3</f>
+        <v>31.047000000000001</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
         <v>0.12130000000000001</v>
       </c>
     </row>

</xml_diff>